<commit_message>
update modules/core: mod       11 files
</commit_message>
<xml_diff>
--- a/starter/src/main/resources/static/excel/team_member.xlsx
+++ b/starter/src/main/resources/static/excel/team_member.xlsx
@@ -47,7 +47,7 @@
     <t>座位号</t>
   </si>
   <si>
-    <t>电话</t>
+    <t>分机号</t>
   </si>
   <si>
     <t>test0</t>
@@ -594,7 +594,7 @@
     </border>
   </borders>
   <cellStyleXfs count="49">
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -746,7 +746,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1288,7 +1288,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="6"/>

</xml_diff>

<commit_message>
update starter/src: mod        2 files
</commit_message>
<xml_diff>
--- a/starter/src/main/resources/static/excel/team_member.xlsx
+++ b/starter/src/main/resources/static/excel/team_member.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>昵称</t>
   </si>
@@ -44,6 +44,9 @@
     <t>职位</t>
   </si>
   <si>
+    <t>部门</t>
+  </si>
+  <si>
     <t>座位号</t>
   </si>
   <si>
@@ -59,6 +62,9 @@
     <t>CEO</t>
   </si>
   <si>
+    <t>管理部</t>
+  </si>
+  <si>
     <t>test1</t>
   </si>
   <si>
@@ -68,6 +74,9 @@
     <t>CTO</t>
   </si>
   <si>
+    <t>设计部</t>
+  </si>
+  <si>
     <t>test2</t>
   </si>
   <si>
@@ -77,10 +86,16 @@
     <t>member</t>
   </si>
   <si>
+    <t>开发部</t>
+  </si>
+  <si>
     <t>test3</t>
   </si>
   <si>
     <t>103@email.com</t>
+  </si>
+  <si>
+    <t>客服部</t>
   </si>
   <si>
     <t>test4</t>
@@ -1285,18 +1300,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="7" width="20" customWidth="1"/>
+    <col min="1" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" spans="1:7">
+    <row r="1" ht="21" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1318,13 +1333,16 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" spans="1:7">
+    <row r="2" s="1" customFormat="1" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="1">
         <v>18888888000</v>
@@ -1333,21 +1351,24 @@
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="G2" s="1">
         <v>0</v>
       </c>
+      <c r="H2" s="1">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" s="1" customFormat="1" spans="1:7">
+    <row r="3" s="1" customFormat="1" spans="1:8">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1">
         <v>18800000001</v>
@@ -1356,21 +1377,24 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="G3" s="1">
         <v>1</v>
       </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" s="1" customFormat="1" spans="1:7">
+    <row r="4" s="1" customFormat="1" spans="1:8">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" s="1">
         <v>18800000002</v>
@@ -1379,21 +1403,24 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2</v>
+        <v>18</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="G4" s="1">
         <v>2</v>
       </c>
+      <c r="H4" s="1">
+        <v>2</v>
+      </c>
     </row>
-    <row r="5" s="1" customFormat="1" spans="1:7">
+    <row r="5" s="1" customFormat="1" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C5" s="1">
         <v>18800000003</v>
@@ -1402,21 +1429,24 @@
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1">
-        <v>3</v>
+        <v>18</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="G5" s="1">
         <v>3</v>
       </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" s="1" customFormat="1" spans="1:7">
+    <row r="6" s="1" customFormat="1" spans="1:8">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="C6" s="1">
         <v>18800000004</v>
@@ -1425,21 +1455,24 @@
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="1">
-        <v>4</v>
+        <v>18</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="G6" s="1">
         <v>4</v>
       </c>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
     </row>
-    <row r="7" s="1" customFormat="1" spans="1:7">
+    <row r="7" s="1" customFormat="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1">
         <v>18800000005</v>
@@ -1448,12 +1481,15 @@
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1">
+        <v>18</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="1">
         <v>5</v>
       </c>
-      <c r="G7" s="1">
+      <c r="H7" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update starter/src: mod        6 del        1 files
</commit_message>
<xml_diff>
--- a/starter/src/main/resources/static/excel/team_member.xlsx
+++ b/starter/src/main/resources/static/excel/team_member.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17260"/>
+    <workbookView windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="member" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>昵称</t>
   </si>
@@ -83,7 +83,7 @@
     <t>102@email.com</t>
   </si>
   <si>
-    <t>member</t>
+    <t>部门经理</t>
   </si>
   <si>
     <t>开发部门</t>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>104@email.com</t>
+  </si>
+  <si>
+    <t>员工</t>
   </si>
   <si>
     <t>test5</t>
@@ -1303,7 +1306,7 @@
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="6" outlineLevelCol="7"/>
@@ -1455,7 +1458,7 @@
         <v>4</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>22</v>
@@ -1469,10 +1472,10 @@
     </row>
     <row r="7" s="1" customFormat="1" spans="1:8">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" s="1">
         <v>18800000005</v>
@@ -1481,7 +1484,7 @@
         <v>5</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>22</v>

</xml_diff>